<commit_message>
#3 cover with test copying images - note: image is copied excatly how it should, but our assertions doesn't check images - todo
</commit_message>
<xml_diff>
--- a/tests/integration/data/Renderer012-ForEach-special/expected.xlsx
+++ b/tests/integration/data/Renderer012-ForEach-special/expected.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="24580" windowHeight="14620" activeTab="2"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="27795" windowHeight="16440" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet sheetId="1" name="Most common for each" state="visible" r:id="rId4"/>
@@ -225,6 +225,251 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>923925</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>448088</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="0" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>923925</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>448088</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="0" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>923925</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>448088</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="0" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>923925</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>448088</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="0" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>923925</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>448088</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="0" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -530,10 +775,10 @@
       <selection activeCell="Q1" sqref="Q1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.35" customHeight="1"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="10" width="10" customWidth="1"/>
-    <col min="11" max="16" width="13.6328125" customWidth="1"/>
+    <col min="11" max="16" width="13.5703125" customWidth="1"/>
     <col min="17" max="18" width="10" customWidth="1"/>
   </cols>
   <sheetData>
@@ -900,9 +1145,9 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.35" customHeight="1"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16" width="16.54296875" customWidth="1"/>
+    <col min="1" max="16" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -1309,11 +1554,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100"/>
+    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
+      <selection activeCell="B20" sqref="B20"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.35" customHeight="1"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="28.453125" customWidth="1"/>
+    <col min="1" max="3" width="28.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -1441,6 +1688,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1448,11 +1696,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100"/>
+    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
+      <selection activeCell="B20" sqref="B20"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.35" customHeight="1"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="28.453125" customWidth="1"/>
+    <col min="1" max="3" width="28.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -1579,6 +1829,7 @@
     <row r="24" spans="1:1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1586,11 +1837,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100"/>
+    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
+      <selection activeCell="B20" sqref="B20"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.35" customHeight="1"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="28.453125" customWidth="1"/>
+    <col min="1" max="3" width="28.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -1718,6 +1971,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1725,11 +1979,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100"/>
+    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
+      <selection activeCell="B20" sqref="B20"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.35" customHeight="1"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="28.453125" customWidth="1"/>
+    <col min="1" max="3" width="28.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -1857,6 +2113,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1864,11 +2121,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100"/>
+    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
+      <selection activeCell="B20" sqref="B20"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.35" customHeight="1"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="28.453125" customWidth="1"/>
+    <col min="1" max="2" width="28.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -1882,5 +2141,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>